<commit_message>
Fix initial state when there are no product cbs to be registered
</commit_message>
<xml_diff>
--- a/coleta_cb.xlsx
+++ b/coleta_cb.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Taquaral" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="72">
   <si>
     <t xml:space="preserve">SAVEGNAGO TAQUARAL</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t xml:space="preserve">massa de tomate </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Computador (5Kg)</t>
   </si>
   <si>
     <t xml:space="preserve">2º TURNO: 12h às 14h</t>
@@ -465,7 +468,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -531,6 +534,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -611,24 +618,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FF00FF00"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G17" activeCellId="1" sqref="A7:F25 G17"/>
+      <selection pane="bottomLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.65234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="35.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="29.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="43.9"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -763,10 +771,21 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
+      <c r="A7" s="9" t="n">
+        <v>12345467</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="10" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="E7" s="9"/>
+      <c r="F7" s="10"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="9"/>
@@ -861,7 +880,7 @@
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
@@ -872,7 +891,7 @@
         <v>7898247780297</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C24" s="9" t="n">
         <v>5</v>
@@ -887,7 +906,7 @@
         <v>7898080640611</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C25" s="9" t="n">
         <v>7</v>
@@ -2323,7 +2342,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFFF0000"/>
     <pageSetUpPr fitToPage="false"/>
@@ -2333,20 +2352,20 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D18" activeCellId="0" sqref="A7:F25"/>
+      <selection pane="bottomLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.65234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="39.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="30.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="13.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="13.24"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -2430,12 +2449,12 @@
         <v>7898215151708</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C4" s="9" t="n">
         <v>26</v>
       </c>
-      <c r="D4" s="9" t="b">
+      <c r="D4" s="10" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -2450,12 +2469,12 @@
         <v>12240900</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C5" s="9" t="n">
         <v>2</v>
       </c>
-      <c r="D5" s="9" t="b">
+      <c r="D5" s="10" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -2465,12 +2484,12 @@
         <v>7891107101621</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C6" s="9" t="n">
         <v>3</v>
       </c>
-      <c r="D6" s="9" t="b">
+      <c r="D6" s="10" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -4270,29 +4289,29 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D19" activeCellId="0" sqref="A7:F25"/>
+      <selection pane="bottomLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.65234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="13.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="13.24"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -4376,12 +4395,12 @@
         <v>7896894900013</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C4" s="9" t="n">
         <v>10</v>
       </c>
-      <c r="D4" s="9" t="b">
+      <c r="D4" s="10" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -4397,12 +4416,12 @@
         <v>7896051111016</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C5" s="9" t="n">
         <v>11</v>
       </c>
-      <c r="D5" s="9" t="b">
+      <c r="D5" s="10" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -4494,7 +4513,7 @@
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
@@ -4510,7 +4529,7 @@
         <v>7891048050668</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C23" s="9" t="n">
         <v>10</v>
@@ -5931,7 +5950,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FF00FF00"/>
     <pageSetUpPr fitToPage="false"/>
@@ -5941,20 +5960,20 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D21" activeCellId="0" sqref="A7:F25"/>
+      <selection pane="bottomLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.65234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="22.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="22.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="13.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="13.24"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -6038,7 +6057,7 @@
         <v>7896584300079</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C4" s="9" t="n">
         <v>7</v>
@@ -6058,7 +6077,7 @@
         <v>7898215151708</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C5" s="9" t="n">
         <v>4</v>
@@ -6073,7 +6092,7 @@
         <v>7896036090244</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C6" s="9" t="n">
         <v>10</v>
@@ -6088,12 +6107,12 @@
         <v>7896894900068</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C7" s="9" t="n">
         <v>2</v>
       </c>
-      <c r="D7" s="10" t="b">
+      <c r="D7" s="17" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -6228,16 +6247,16 @@
       <c r="A29" s="9"/>
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
-      <c r="D29" s="10" t="b">
+      <c r="D29" s="17" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="17"/>
-      <c r="B30" s="17"/>
-      <c r="C30" s="17"/>
-      <c r="D30" s="17"/>
+      <c r="A30" s="18"/>
+      <c r="B30" s="18"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="9"/>
@@ -6501,7 +6520,7 @@
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B74" s="7"/>
       <c r="C74" s="7"/>
@@ -6512,7 +6531,7 @@
         <v>7896584300352</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C75" s="9" t="n">
         <v>5</v>
@@ -6527,7 +6546,7 @@
         <v>7896584300079</v>
       </c>
       <c r="B76" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C76" s="9" t="n">
         <v>6</v>
@@ -6542,7 +6561,7 @@
         <v>7891032014621</v>
       </c>
       <c r="B77" s="9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C77" s="9" t="n">
         <v>1</v>
@@ -6557,7 +6576,7 @@
         <v>7896005275399</v>
       </c>
       <c r="B78" s="9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C78" s="9" t="n">
         <v>8</v>
@@ -6572,7 +6591,7 @@
         <v>7897517206338</v>
       </c>
       <c r="B79" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C79" s="9" t="n">
         <v>2</v>
@@ -6587,7 +6606,7 @@
         <v>7896080841403</v>
       </c>
       <c r="B80" s="9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C80" s="9" t="n">
         <v>1</v>
@@ -6602,7 +6621,7 @@
         <v>7896894900013</v>
       </c>
       <c r="B81" s="9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C81" s="9" t="n">
         <v>2</v>
@@ -6617,7 +6636,7 @@
         <v>7896060401818</v>
       </c>
       <c r="B82" s="9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C82" s="9" t="n">
         <v>1</v>
@@ -6632,7 +6651,7 @@
         <v>7896104996393</v>
       </c>
       <c r="B83" s="9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C83" s="9" t="n">
         <v>1</v>
@@ -6647,7 +6666,7 @@
         <v>7896045110582</v>
       </c>
       <c r="B84" s="9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C84" s="9" t="n">
         <v>1</v>
@@ -6662,7 +6681,7 @@
         <v>7891022638004</v>
       </c>
       <c r="B85" s="9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C85" s="9" t="n">
         <v>3</v>
@@ -6677,7 +6696,7 @@
         <v>7891095300372</v>
       </c>
       <c r="B86" s="9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C86" s="9" t="n">
         <v>1</v>
@@ -6692,7 +6711,7 @@
         <v>7622210571816</v>
       </c>
       <c r="B87" s="9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C87" s="9" t="n">
         <v>3</v>
@@ -6707,7 +6726,7 @@
         <v>7891048050668</v>
       </c>
       <c r="B88" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C88" s="9" t="n">
         <v>4</v>
@@ -6722,7 +6741,7 @@
         <v>7891000376881</v>
       </c>
       <c r="B89" s="9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C89" s="9" t="n">
         <v>2</v>
@@ -6737,7 +6756,7 @@
         <v>7891107101621</v>
       </c>
       <c r="B90" s="9" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C90" s="9" t="n">
         <v>1</v>
@@ -6752,7 +6771,7 @@
         <v>7986051111016</v>
       </c>
       <c r="B91" s="9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C91" s="9" t="n">
         <v>1</v>
@@ -6767,7 +6786,7 @@
         <v>7891528029498</v>
       </c>
       <c r="B92" s="9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C92" s="9" t="n">
         <v>1</v>
@@ -6782,7 +6801,7 @@
         <v>7891176117455</v>
       </c>
       <c r="B93" s="9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C93" s="9" t="n">
         <v>6</v>
@@ -7772,32 +7791,33 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFFF0000"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:AB996"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7:F25"/>
+      <selection pane="bottomLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.65234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="41.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="37.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="12.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="13.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="41.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="13.24"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -7887,7 +7907,7 @@
         <v>7896005202074</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
@@ -7909,7 +7929,7 @@
         <v>7896200115346</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
@@ -7926,7 +7946,7 @@
         <v>7898215151708</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
@@ -7943,7 +7963,7 @@
         <v>7896256601848</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C7" s="9" t="n">
         <v>12</v>
@@ -7952,7 +7972,7 @@
       <c r="E7" s="9" t="n">
         <v>12</v>
       </c>
-      <c r="F7" s="9" t="b">
+      <c r="F7" s="10" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -7963,7 +7983,7 @@
         <v>7896005286593</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C8" s="9" t="n">
         <v>23</v>
@@ -7972,7 +7992,7 @@
       <c r="E8" s="9" t="n">
         <v>23</v>
       </c>
-      <c r="F8" s="9" t="b">
+      <c r="F8" s="10" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -7982,7 +8002,7 @@
         <v>7896894900013</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C9" s="9" t="n">
         <v>4</v>
@@ -8001,7 +8021,7 @@
         <v>7896527702618</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C10" s="9" t="n">
         <v>2</v>
@@ -8020,7 +8040,7 @@
         <v>7896356800035</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C11" s="9" t="n">
         <v>4</v>
@@ -8037,7 +8057,7 @@
         <v>7896006744115</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C12" s="9" t="n">
         <v>7</v>
@@ -8056,7 +8076,7 @@
         <v>7896901200143</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C13" s="9" t="n">
         <v>2</v>
@@ -8073,7 +8093,7 @@
         <v>7896036090244</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C14" s="9" t="n">
         <v>3</v>
@@ -8090,7 +8110,7 @@
         <v>7896235353331</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C15" s="9" t="n">
         <v>2</v>
@@ -8107,7 +8127,7 @@
         <v>7896098909782</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C16" s="9" t="n">
         <v>1</v>
@@ -8124,7 +8144,7 @@
         <v>7896036099544</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C17" s="9" t="n">
         <v>2</v>
@@ -8141,7 +8161,7 @@
         <v>7896235353454</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C18" s="9" t="n">
         <v>1</v>
@@ -8158,7 +8178,7 @@
         <v>7896584300246</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C19" s="9" t="n">
         <v>3</v>
@@ -8175,7 +8195,7 @@
         <v>7896405105210</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C20" s="9" t="n">
         <v>2</v>
@@ -8192,7 +8212,7 @@
         <v>7896098900253</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C21" s="9" t="n">
         <v>4</v>
@@ -8209,7 +8229,7 @@
         <v>7896327511281</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C22" s="9" t="n">
         <v>2</v>
@@ -8226,14 +8246,14 @@
         <v>7891203068637</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C23" s="9" t="n">
         <v>1</v>
       </c>
       <c r="D23" s="9"/>
       <c r="E23" s="9"/>
-      <c r="F23" s="9" t="b">
+      <c r="F23" s="10" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -8243,14 +8263,14 @@
         <v>7894000010014</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C24" s="9" t="n">
         <v>2</v>
       </c>
       <c r="D24" s="9"/>
       <c r="E24" s="9"/>
-      <c r="F24" s="9" t="b">
+      <c r="F24" s="10" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -8260,25 +8280,34 @@
         <v>7896527700898</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C25" s="9" t="n">
         <v>1</v>
       </c>
       <c r="D25" s="9"/>
       <c r="E25" s="9"/>
-      <c r="F25" s="9" t="b">
+      <c r="F25" s="10" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="9"/>
-      <c r="B26" s="9"/>
-      <c r="C26" s="9"/>
+      <c r="A26" s="9" t="n">
+        <v>12345467</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26" s="9" t="n">
+        <v>1</v>
+      </c>
       <c r="D26" s="9"/>
       <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
+      <c r="F26" s="10" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="9"/>
@@ -8329,12 +8358,12 @@
       <c r="F32" s="9"/>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="17"/>
-      <c r="B33" s="17"/>
-      <c r="C33" s="17"/>
-      <c r="D33" s="17"/>
-      <c r="E33" s="17"/>
-      <c r="F33" s="17"/>
+      <c r="A33" s="18"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="9"/>
@@ -9867,7 +9896,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FF00FF00"/>
     <pageSetUpPr fitToPage="false"/>
@@ -9877,10 +9906,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F23" activeCellId="0" sqref="A7:F25"/>
+      <selection pane="bottomLeft" activeCell="F23" activeCellId="0" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.65234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="29.25"/>
@@ -9889,7 +9918,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -9973,12 +10002,12 @@
         <v>7891910000197</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C4" s="9" t="n">
         <v>8</v>
       </c>
-      <c r="D4" s="9" t="b">
+      <c r="D4" s="10" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -9993,12 +10022,12 @@
         <v>7896327512615</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C5" s="9" t="n">
         <v>2</v>
       </c>
-      <c r="D5" s="9" t="b">
+      <c r="D5" s="10" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -10008,12 +10037,12 @@
         <v>7896005286593</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C6" s="9" t="n">
         <v>18</v>
       </c>
-      <c r="D6" s="9" t="b">
+      <c r="D6" s="10" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -10023,12 +10052,12 @@
         <v>7897664171701</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C7" s="9" t="n">
         <v>4</v>
       </c>
-      <c r="D7" s="9" t="b">
+      <c r="D7" s="10" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>

</xml_diff>